<commit_message>
Adding Add a member project
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kokila/eclipse-workspace/addMember/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kokila/eclipse-workspace/addMemberNew/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08D6464-3D28-F744-A456-23DA9EE40D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778668CB-0E72-B245-AE3E-40D1C9E56CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="3240" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{153DDED3-5CD1-4443-A0AC-B388A5BA5E66}"/>
+    <workbookView xWindow="7800" yWindow="3240" windowWidth="28040" windowHeight="17440" xr2:uid="{153DDED3-5CD1-4443-A0AC-B388A5BA5E66}"/>
   </bookViews>
   <sheets>
-    <sheet name="Member Contact" sheetId="1" r:id="rId1"/>
+    <sheet name="MemberContact" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
   <si>
     <t>Password</t>
   </si>
@@ -50,10 +50,229 @@
     <t>itoddev96</t>
   </si>
   <si>
-    <t>test@test.com</t>
-  </si>
-  <si>
-    <t>bcd1234</t>
+    <t>Salutation</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Judge</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>NickName</t>
+  </si>
+  <si>
+    <t>Suffix</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Esq.</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Phone1</t>
+  </si>
+  <si>
+    <t>Phone2</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Latino</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>456-763-1097</t>
+  </si>
+  <si>
+    <t>123-456-7890</t>
+  </si>
+  <si>
+    <t>708-567-2146</t>
+  </si>
+  <si>
+    <t>543-189-9065</t>
+  </si>
+  <si>
+    <t>contracosta@abc19.com</t>
+  </si>
+  <si>
+    <t>15,abc street</t>
+  </si>
+  <si>
+    <t>Suite101</t>
+  </si>
+  <si>
+    <t>Wilmington</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>www.avf.com</t>
+  </si>
+  <si>
+    <t>Attorney</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>MemberPwd</t>
+  </si>
+  <si>
+    <t>high12</t>
+  </si>
+  <si>
+    <t>MemberId</t>
+  </si>
+  <si>
+    <t>IMIS</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>NotesText</t>
+  </si>
+  <si>
+    <t>This is a sample message for private notes.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>03/18/1990</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>ContactPrefference</t>
+  </si>
+  <si>
+    <t>MagazinePrefference</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>19804</t>
+  </si>
+  <si>
+    <t>165489</t>
+  </si>
+  <si>
+    <t>EventBroadcastPrefference</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>CommitteBroadcastPrefference</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>MailingOption</t>
+  </si>
+  <si>
+    <t>StudentMentor</t>
+  </si>
+  <si>
+    <t>AttorneyMentor</t>
+  </si>
+  <si>
+    <t>MentorToStudent</t>
+  </si>
+  <si>
+    <t>MentorToAttorney</t>
+  </si>
+  <si>
+    <t>PublishNameOnline</t>
+  </si>
+  <si>
+    <t>PublishNamePrint</t>
+  </si>
+  <si>
+    <t>PublishEmailOnline</t>
+  </si>
+  <si>
+    <t>PublishEmailPrint</t>
+  </si>
+  <si>
+    <t>PublishPhoneOnline</t>
+  </si>
+  <si>
+    <t>PublishPhonePrint</t>
+  </si>
+  <si>
+    <t>PublishPhotoOnline</t>
+  </si>
+  <si>
+    <t>PublishPhotoPrint</t>
+  </si>
+  <si>
+    <t>PublishBioOnline</t>
+  </si>
+  <si>
+    <t>PublishBioPrint</t>
   </si>
 </sst>
 </file>
@@ -75,12 +294,10 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,17 +317,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,22 +642,327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B3474E-A8B0-BB44-A44D-131CFF0E3398}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AS2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AS3" sqref="AS3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5CA3A1-BDCE-8049-9805-121E142C3110}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,18 +986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{93FE374E-3CBF-BD43-8981-917A72BC7BEF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned the codes for simplification.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kokila/eclipse-workspace/addMemberNew/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778668CB-0E72-B245-AE3E-40D1C9E56CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063952EA-90B8-B942-B3D7-6F18ED088ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="3240" windowWidth="28040" windowHeight="17440" xr2:uid="{153DDED3-5CD1-4443-A0AC-B388A5BA5E66}"/>
   </bookViews>
   <sheets>
     <sheet name="MemberContact" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="MembershipCategories" sheetId="3" r:id="rId2"/>
+    <sheet name="LanguageCategories" sheetId="4" r:id="rId3"/>
+    <sheet name="PaymentCategory" sheetId="5" r:id="rId4"/>
+    <sheet name="Login" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="113">
   <si>
     <t>Password</t>
   </si>
@@ -149,9 +152,6 @@
     <t>543-189-9065</t>
   </si>
   <si>
-    <t>contracosta@abc19.com</t>
-  </si>
-  <si>
     <t>15,abc street</t>
   </si>
   <si>
@@ -215,9 +215,6 @@
     <t>19804</t>
   </si>
   <si>
-    <t>165489</t>
-  </si>
-  <si>
     <t>EventBroadcastPrefference</t>
   </si>
   <si>
@@ -273,13 +270,121 @@
   </si>
   <si>
     <t>PublishBioPrint</t>
+  </si>
+  <si>
+    <t>MemberCategory</t>
+  </si>
+  <si>
+    <t>Chinese,Tamil,Hindi,English</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>DonationInformation</t>
+  </si>
+  <si>
+    <t>JFK &amp; JD Scholarship|200,member_renewal_cont_nc|100</t>
+  </si>
+  <si>
+    <t>ProductServices</t>
+  </si>
+  <si>
+    <t>LAW_Test 1|2|150</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>PaymentNotes</t>
+  </si>
+  <si>
+    <t>Test Payment Note.</t>
+  </si>
+  <si>
+    <t>DateAdmitted</t>
+  </si>
+  <si>
+    <t>02/15/2002</t>
+  </si>
+  <si>
+    <t>03/18/2002</t>
+  </si>
+  <si>
+    <t>DateFirstAdmittedToState</t>
+  </si>
+  <si>
+    <t>SameMailinfInfo</t>
+  </si>
+  <si>
+    <t>OfficePhone</t>
+  </si>
+  <si>
+    <t>OfficeFax</t>
+  </si>
+  <si>
+    <t>376-287-1954</t>
+  </si>
+  <si>
+    <t>532-326-1785</t>
+  </si>
+  <si>
+    <t>Email1</t>
+  </si>
+  <si>
+    <t>Email2</t>
+  </si>
+  <si>
+    <t>OfficeAddress1</t>
+  </si>
+  <si>
+    <t>OfficeAddress2</t>
+  </si>
+  <si>
+    <t>acv@costa.com</t>
+  </si>
+  <si>
+    <t>189,car strret</t>
+  </si>
+  <si>
+    <t>OfficeAddressCity</t>
+  </si>
+  <si>
+    <t>OfficeAddressState</t>
+  </si>
+  <si>
+    <t>OfficeAddressZipcode</t>
+  </si>
+  <si>
+    <t>OfficeAddressCounty</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Fenton</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>38764</t>
+  </si>
+  <si>
+    <t>1654828</t>
+  </si>
+  <si>
+    <t>contracosta@abcd12191.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -296,6 +401,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -317,10 +436,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -328,8 +448,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -642,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B3474E-A8B0-BB44-A44D-131CFF0E3398}">
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:BF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AS3" sqref="AS3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,9 +800,17 @@
     <col min="42" max="42" width="22.5" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="52" width="18.83203125" customWidth="1"/>
+    <col min="53" max="53" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -743,79 +875,118 @@
         <v>30</v>
       </c>
       <c r="V1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" t="s">
-        <v>48</v>
-      </c>
       <c r="Z1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AA1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB1" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" t="s">
-        <v>56</v>
-      </c>
       <c r="AC1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD1" t="s">
         <v>60</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>62</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG1" t="s">
         <v>64</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AR1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AS1" s="4" t="s">
-        <v>78</v>
+      <c r="AT1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BB1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BE1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF1" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -835,7 +1006,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>31</v>
@@ -844,7 +1015,7 @@
         <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>33</v>
@@ -858,98 +1029,183 @@
       <c r="N2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="X2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AE2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AG2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AI2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AJ2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AK2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AM2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AO2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AP2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AQ2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AR2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AS2" s="1" t="s">
-        <v>63</v>
+      <c r="AT2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{89D51416-45DF-7940-9BA1-A5637FDE60A2}"/>
+    <hyperlink ref="AW2" r:id="rId2" xr:uid="{F032B9C3-7133-5648-A3C3-FC860426EA47}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03DA1B6-4441-3A42-9399-5D602A59A513}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -957,12 +1213,75 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FDC337-4B70-1C40-BE92-C568CABCC105}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE6E666-3F57-C949-A0DC-5AC82CA6FA18}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5CA3A1-BDCE-8049-9805-121E142C3110}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>